<commit_message>
Fix tunel pvs names
</commit_message>
<xml_diff>
--- a/etc/SiriusAmbTempPVs.xlsx
+++ b/etc/SiriusAmbTempPVs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25809"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cnpemcamp.sharepoint.com/sites/GrupoAutomaoeSoftware/Documentos Compartilhados/Estabilidade do Feixe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D81EA5B-80E5-4B8E-868A-A2DB226221B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D77AEDA-883D-48F9-B084-CCD6C476F068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="4" xr2:uid="{CC45857C-43CA-4FE8-B43A-A3E2BD5298BB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{CC45857C-43CA-4FE8-B43A-A3E2BD5298BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Hall" sheetId="5" r:id="rId1"/>
@@ -2625,7 +2625,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="235">
+  <cellXfs count="236">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3316,13 +3316,16 @@
     <xf numFmtId="0" fontId="7" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="15" fillId="37" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="37" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -14759,8 +14762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AC98F7D-7F2B-4614-9245-C95CA7A32884}">
   <dimension ref="A1:W55"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16562,8 +16565,8 @@
         <v>27</v>
       </c>
       <c r="J29" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-39IW:AC-PT100-:Temperature-Mon</v>
+        <f>IF(G29="-",C29&amp;"-"&amp;D29&amp;":"&amp;E29&amp;"-"&amp;F29&amp;":"&amp;H29&amp;"-"&amp;I29,C29&amp;"-"&amp;D29&amp;":"&amp;E29&amp;"-"&amp;F29&amp;G29&amp;":"&amp;H29&amp;"-"&amp;I29)</f>
+        <v>TU-39IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="K29" s="159" t="s">
         <v>411</v>
@@ -16624,14 +16627,14 @@
         <v>27</v>
       </c>
       <c r="J30" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-40EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" ref="J30:J55" si="1">IF(G30="-",C30&amp;"-"&amp;D30&amp;":"&amp;E30&amp;"-"&amp;F30&amp;":"&amp;H30&amp;"-"&amp;I30,C30&amp;"-"&amp;D30&amp;":"&amp;E30&amp;"-"&amp;F30&amp;G30&amp;":"&amp;H30&amp;"-"&amp;I30)</f>
+        <v>TU-40EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="K30" s="159" t="s">
         <v>413</v>
       </c>
       <c r="L30" s="129" t="str">
-        <f t="shared" ref="L30:L35" si="1">K30&amp;"_ST_614_"&amp;MID($B30,8,2)&amp;"_"&amp;IF(MID($B30,11,1)="0", MID($B30,12,1), MID($B30,11,2))&amp;".val"</f>
+        <f t="shared" ref="L30:L35" si="2">K30&amp;"_ST_614_"&amp;MID($B30,8,2)&amp;"_"&amp;IF(MID($B30,11,1)="0", MID($B30,12,1), MID($B30,11,2))&amp;".val"</f>
         <v>TEAMB02_ST_614_17_2.val</v>
       </c>
       <c r="M30" s="130" t="s">
@@ -16649,7 +16652,7 @@
         <v>31</v>
       </c>
       <c r="S30" s="132" t="str">
-        <f t="shared" ref="S30:S54" si="2">L30</f>
+        <f t="shared" ref="S30:S54" si="3">L30</f>
         <v>TEAMB02_ST_614_17_2.val</v>
       </c>
       <c r="T30" s="128" t="s">
@@ -16686,14 +16689,14 @@
         <v>27</v>
       </c>
       <c r="J31" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-41IW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-41IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="K31" s="159" t="s">
         <v>415</v>
       </c>
       <c r="L31" s="129" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB03_ST_614_17_4.val</v>
       </c>
       <c r="M31" s="130" t="s">
@@ -16711,7 +16714,7 @@
         <v>31</v>
       </c>
       <c r="S31" s="132" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TEAMB03_ST_614_17_4.val</v>
       </c>
       <c r="T31" s="128" t="s">
@@ -16748,14 +16751,14 @@
         <v>27</v>
       </c>
       <c r="J32" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-41EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-41EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="K32" s="159" t="s">
         <v>417</v>
       </c>
       <c r="L32" s="129" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB04_ST_614_17_5.val</v>
       </c>
       <c r="M32" s="130" t="s">
@@ -16773,7 +16776,7 @@
         <v>31</v>
       </c>
       <c r="S32" s="132" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TEAMB04_ST_614_17_5.val</v>
       </c>
       <c r="T32" s="128" t="s">
@@ -16810,14 +16813,14 @@
         <v>27</v>
       </c>
       <c r="J33" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-42IW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-42IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="K33" s="159" t="s">
         <v>419</v>
       </c>
       <c r="L33" s="129" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB05_ST_614_17_7.val</v>
       </c>
       <c r="M33" s="130" t="s">
@@ -16835,7 +16838,7 @@
         <v>31</v>
       </c>
       <c r="S33" s="132" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TEAMB05_ST_614_17_7.val</v>
       </c>
       <c r="T33" s="128" t="s">
@@ -16872,14 +16875,14 @@
         <v>27</v>
       </c>
       <c r="J34" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-43EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-43EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="K34" s="159" t="s">
         <v>421</v>
       </c>
       <c r="L34" s="129" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB06_ST_614_17_8.val</v>
       </c>
       <c r="M34" s="130" t="s">
@@ -16897,7 +16900,7 @@
         <v>31</v>
       </c>
       <c r="S34" s="132" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TEAMB06_ST_614_17_8.val</v>
       </c>
       <c r="T34" s="128" t="s">
@@ -16934,14 +16937,14 @@
         <v>27</v>
       </c>
       <c r="J35" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-44IW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-44IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="K35" s="159" t="s">
         <v>423</v>
       </c>
       <c r="L35" s="129" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB07_ST_614_17_9.val</v>
       </c>
       <c r="M35" s="130" t="s">
@@ -16959,7 +16962,7 @@
         <v>31</v>
       </c>
       <c r="S35" s="132" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TEAMB07_ST_614_17_9.val</v>
       </c>
       <c r="T35" s="128" t="s">
@@ -16996,8 +16999,8 @@
         <v>27</v>
       </c>
       <c r="J36" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-44EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-44EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="K36" s="159" t="s">
         <v>425</v>
@@ -17056,8 +17059,8 @@
         <v>27</v>
       </c>
       <c r="J37" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-3944:AC-PT101-:MeanTemperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-3944:AC-PT101:MeanTemperature-Mon</v>
       </c>
       <c r="K37" s="159"/>
       <c r="L37" s="129" t="s">
@@ -17113,8 +17116,8 @@
         <v>27</v>
       </c>
       <c r="J38" s="221" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-45IW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-45IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="K38" s="159" t="s">
         <v>411</v>
@@ -17138,7 +17141,7 @@
         <v>31</v>
       </c>
       <c r="S38" s="138" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TEAMB01_ST_614_19_1.val</v>
       </c>
       <c r="T38" s="134" t="s">
@@ -17175,14 +17178,14 @@
         <v>27</v>
       </c>
       <c r="J39" s="221" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-46EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-46EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="K39" s="159" t="s">
         <v>413</v>
       </c>
       <c r="L39" s="135" t="str">
-        <f t="shared" ref="L39:L45" si="3">K39&amp;"_ST_614_"&amp;MID($B39,8,2)&amp;"_"&amp;IF(MID($B39,11,1)="0", MID($B39,12,1), MID($B39,11,2))&amp;".val"</f>
+        <f t="shared" ref="L39:L45" si="4">K39&amp;"_ST_614_"&amp;MID($B39,8,2)&amp;"_"&amp;IF(MID($B39,11,1)="0", MID($B39,12,1), MID($B39,11,2))&amp;".val"</f>
         <v>TEAMB02_ST_614_19_2.val</v>
       </c>
       <c r="M39" s="136" t="s">
@@ -17200,7 +17203,7 @@
         <v>31</v>
       </c>
       <c r="S39" s="138" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TEAMB02_ST_614_19_2.val</v>
       </c>
       <c r="T39" s="134" t="s">
@@ -17237,14 +17240,14 @@
         <v>27</v>
       </c>
       <c r="J40" s="221" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-47IW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-47IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="K40" s="159" t="s">
         <v>415</v>
       </c>
       <c r="L40" s="135" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>TEAMB03_ST_614_19_4.val</v>
       </c>
       <c r="M40" s="136" t="s">
@@ -17262,7 +17265,7 @@
         <v>31</v>
       </c>
       <c r="S40" s="138" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TEAMB03_ST_614_19_4.val</v>
       </c>
       <c r="T40" s="134" t="s">
@@ -17299,14 +17302,14 @@
         <v>27</v>
       </c>
       <c r="J41" s="221" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-47EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-47EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="K41" s="159" t="s">
         <v>417</v>
       </c>
       <c r="L41" s="135" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>TEAMB04_ST_614_19_5.val</v>
       </c>
       <c r="M41" s="136" t="s">
@@ -17324,7 +17327,7 @@
         <v>31</v>
       </c>
       <c r="S41" s="138" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TEAMB04_ST_614_19_5.val</v>
       </c>
       <c r="T41" s="134" t="s">
@@ -17361,14 +17364,14 @@
         <v>27</v>
       </c>
       <c r="J42" s="221" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-48IW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-48IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="K42" s="159" t="s">
         <v>419</v>
       </c>
       <c r="L42" s="135" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>TEAMB05_ST_614_19_7.val</v>
       </c>
       <c r="M42" s="136" t="s">
@@ -17386,7 +17389,7 @@
         <v>31</v>
       </c>
       <c r="S42" s="138" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TEAMB05_ST_614_19_7.val</v>
       </c>
       <c r="T42" s="134" t="s">
@@ -17415,7 +17418,7 @@
       <c r="F43" s="210" t="s">
         <v>24</v>
       </c>
-      <c r="G43" s="214"/>
+      <c r="G43" s="235"/>
       <c r="H43" s="160" t="s">
         <v>26</v>
       </c>
@@ -17423,14 +17426,14 @@
         <v>27</v>
       </c>
       <c r="J43" s="221" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-49EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-49EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="K43" s="159" t="s">
         <v>421</v>
       </c>
       <c r="L43" s="135" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>TEAMB06_ST_614_19_8.val</v>
       </c>
       <c r="M43" s="136" t="s">
@@ -17448,7 +17451,7 @@
         <v>31</v>
       </c>
       <c r="S43" s="138" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TEAMB06_ST_614_19_8.val</v>
       </c>
       <c r="T43" s="134" t="s">
@@ -17485,14 +17488,14 @@
         <v>27</v>
       </c>
       <c r="J44" s="221" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-50IW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-50IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="K44" s="159" t="s">
         <v>423</v>
       </c>
       <c r="L44" s="135" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>TEAMB07_ST_614_19_9.val</v>
       </c>
       <c r="M44" s="136" t="s">
@@ -17510,7 +17513,7 @@
         <v>31</v>
       </c>
       <c r="S44" s="138" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TEAMB07_ST_614_19_9.val</v>
       </c>
       <c r="T44" s="134" t="s">
@@ -17547,14 +17550,14 @@
         <v>27</v>
       </c>
       <c r="J45" s="221" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-50EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-50EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="K45" s="159" t="s">
         <v>425</v>
       </c>
       <c r="L45" s="135" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>TEAMB08_ST_614_19_10.val</v>
       </c>
       <c r="M45" s="136" t="s">
@@ -17572,7 +17575,7 @@
         <v>31</v>
       </c>
       <c r="S45" s="138" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TEAMB08_ST_614_19_10.val</v>
       </c>
       <c r="T45" s="134" t="s">
@@ -17607,8 +17610,8 @@
         <v>27</v>
       </c>
       <c r="J46" s="221" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-4550:AC-PT100-:MeanTemperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-4550:AC-PT100:MeanTemperature-Mon</v>
       </c>
       <c r="K46" s="159"/>
       <c r="L46" s="135" t="s">
@@ -17664,8 +17667,8 @@
         <v>27</v>
       </c>
       <c r="J47" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-51IW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-51IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="K47" s="159" t="s">
         <v>411</v>
@@ -17689,7 +17692,7 @@
         <v>287</v>
       </c>
       <c r="S47" s="132" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TEAMB01_ST_614_02_1.val</v>
       </c>
       <c r="T47" s="128" t="s">
@@ -17726,14 +17729,14 @@
         <v>27</v>
       </c>
       <c r="J48" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-52EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-52EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="K48" s="159" t="s">
         <v>413</v>
       </c>
       <c r="L48" s="129" t="str">
-        <f t="shared" ref="L48:L54" si="4">K48&amp;"_ST_614_"&amp;MID($B48,8,2)&amp;"_"&amp;IF(MID($B48,11,1)="0", MID($B48,12,1), MID($B48,11,2))&amp;".val"</f>
+        <f t="shared" ref="L48:L54" si="5">K48&amp;"_ST_614_"&amp;MID($B48,8,2)&amp;"_"&amp;IF(MID($B48,11,1)="0", MID($B48,12,1), MID($B48,11,2))&amp;".val"</f>
         <v>TEAMB02_ST_614_02_2.val</v>
       </c>
       <c r="M48" s="130" t="s">
@@ -17751,7 +17754,7 @@
         <v>31</v>
       </c>
       <c r="S48" s="132" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TEAMB02_ST_614_02_2.val</v>
       </c>
       <c r="T48" s="128" t="s">
@@ -17788,14 +17791,14 @@
         <v>27</v>
       </c>
       <c r="J49" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-53IW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-53IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="K49" s="159" t="s">
         <v>415</v>
       </c>
       <c r="L49" s="129" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>TEAMB03_ST_614_02_4.val</v>
       </c>
       <c r="M49" s="130" t="s">
@@ -17813,7 +17816,7 @@
         <v>31</v>
       </c>
       <c r="S49" s="132" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TEAMB03_ST_614_02_4.val</v>
       </c>
       <c r="T49" s="128" t="s">
@@ -17850,14 +17853,14 @@
         <v>27</v>
       </c>
       <c r="J50" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-53EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-53EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="K50" s="159" t="s">
         <v>417</v>
       </c>
       <c r="L50" s="129" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>TEAMB04_ST_614_02_5.val</v>
       </c>
       <c r="M50" s="130" t="s">
@@ -17875,7 +17878,7 @@
         <v>31</v>
       </c>
       <c r="S50" s="132" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TEAMB04_ST_614_02_5.val</v>
       </c>
       <c r="T50" s="128" t="s">
@@ -17912,14 +17915,14 @@
         <v>27</v>
       </c>
       <c r="J51" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-54IW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-54IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="K51" s="159" t="s">
         <v>419</v>
       </c>
       <c r="L51" s="129" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>TEAMB05_ST_614_02_7.val</v>
       </c>
       <c r="M51" s="130" t="s">
@@ -17937,7 +17940,7 @@
         <v>31</v>
       </c>
       <c r="S51" s="132" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TEAMB05_ST_614_02_7.val</v>
       </c>
       <c r="T51" s="128" t="s">
@@ -17974,14 +17977,14 @@
         <v>27</v>
       </c>
       <c r="J52" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-55EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-55EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="K52" s="159" t="s">
         <v>421</v>
       </c>
       <c r="L52" s="129" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>TEAMB06_ST_614_02_8.val</v>
       </c>
       <c r="M52" s="130" t="s">
@@ -17999,7 +18002,7 @@
         <v>31</v>
       </c>
       <c r="S52" s="132" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TEAMB06_ST_614_02_8.val</v>
       </c>
       <c r="T52" s="128" t="s">
@@ -18036,14 +18039,14 @@
         <v>27</v>
       </c>
       <c r="J53" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-56IW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-56IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="K53" s="159" t="s">
         <v>423</v>
       </c>
       <c r="L53" s="129" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>TEAMB07_ST_614_02_9.val</v>
       </c>
       <c r="M53" s="130" t="s">
@@ -18061,7 +18064,7 @@
         <v>31</v>
       </c>
       <c r="S53" s="132" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TEAMB07_ST_614_02_9.val</v>
       </c>
       <c r="T53" s="128" t="s">
@@ -18098,14 +18101,14 @@
         <v>27</v>
       </c>
       <c r="J54" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-56EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-56EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="K54" s="189" t="s">
         <v>425</v>
       </c>
       <c r="L54" s="190" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>TEAMB08_ST_614_02_10.val</v>
       </c>
       <c r="M54" s="191" t="s">
@@ -18123,7 +18126,7 @@
         <v>31</v>
       </c>
       <c r="S54" s="194" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TEAMB08_ST_614_02_10.val</v>
       </c>
       <c r="T54" s="188" t="s">
@@ -18158,8 +18161,8 @@
         <v>27</v>
       </c>
       <c r="J55" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-5156:AC-PT101-:MeanTemperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-5156:AC-PT101:MeanTemperature-Mon</v>
       </c>
       <c r="K55" s="196"/>
       <c r="L55" s="197" t="s">
@@ -18197,8 +18200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1749B5E6-42A0-4EC2-B63B-2AAA50CDAECA}">
   <dimension ref="A1:X73"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="L65" sqref="L65:L73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -20606,8 +20609,8 @@
         <v>411</v>
       </c>
       <c r="L38" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-09IW:AC-PT100-:Temperature-Mon</v>
+        <f>IF(G38="-",C38&amp;"-"&amp;D38&amp;":"&amp;E38&amp;"-"&amp;F38&amp;":"&amp;H38&amp;"-"&amp;J38,C38&amp;"-"&amp;D38&amp;":"&amp;E38&amp;"-"&amp;F38&amp;G38&amp;":"&amp;H38&amp;"-"&amp;J38)</f>
+        <v>TU-09IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="M38" s="151" t="s">
         <v>496</v>
@@ -20668,8 +20671,8 @@
         <v>413</v>
       </c>
       <c r="L39" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-10EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" ref="L39:L73" si="1">IF(G39="-",C39&amp;"-"&amp;D39&amp;":"&amp;E39&amp;"-"&amp;F39&amp;":"&amp;H39&amp;"-"&amp;J39,C39&amp;"-"&amp;D39&amp;":"&amp;E39&amp;"-"&amp;F39&amp;G39&amp;":"&amp;H39&amp;"-"&amp;J39)</f>
+        <v>TU-10EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="M39" s="151" t="s">
         <v>498</v>
@@ -20689,7 +20692,7 @@
         <v>31</v>
       </c>
       <c r="T39" s="153" t="str">
-        <f t="shared" ref="T39:T72" si="1">M39</f>
+        <f t="shared" ref="T39:T72" si="2">M39</f>
         <v>TEAMB02_ST_614_08_2.val</v>
       </c>
       <c r="U39" s="150" t="s">
@@ -20730,8 +20733,8 @@
         <v>415</v>
       </c>
       <c r="L40" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-11IW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-11IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="M40" s="151" t="s">
         <v>500</v>
@@ -20751,7 +20754,7 @@
         <v>31</v>
       </c>
       <c r="T40" s="153" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB03_ST_614_08_4.val</v>
       </c>
       <c r="U40" s="150" t="s">
@@ -20792,8 +20795,8 @@
         <v>417</v>
       </c>
       <c r="L41" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-11EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-11EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="M41" s="151" t="s">
         <v>502</v>
@@ -20813,7 +20816,7 @@
         <v>31</v>
       </c>
       <c r="T41" s="153" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB04_ST_614_08_5.val</v>
       </c>
       <c r="U41" s="150" t="s">
@@ -20854,8 +20857,8 @@
         <v>419</v>
       </c>
       <c r="L42" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-12IW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-12IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="M42" s="151" t="s">
         <v>504</v>
@@ -20875,7 +20878,7 @@
         <v>31</v>
       </c>
       <c r="T42" s="153" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB05_ST_614_08_7.val</v>
       </c>
       <c r="U42" s="150" t="s">
@@ -20916,8 +20919,8 @@
         <v>421</v>
       </c>
       <c r="L43" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-13EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-13EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="M43" s="151" t="s">
         <v>506</v>
@@ -20937,7 +20940,7 @@
         <v>31</v>
       </c>
       <c r="T43" s="153" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB06_ST_614_08_8.val</v>
       </c>
       <c r="U43" s="150" t="s">
@@ -20978,8 +20981,8 @@
         <v>423</v>
       </c>
       <c r="L44" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-14IW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-14IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="M44" s="151" t="s">
         <v>508</v>
@@ -20999,7 +21002,7 @@
         <v>31</v>
       </c>
       <c r="T44" s="153" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB07_ST_614_08_9.val</v>
       </c>
       <c r="U44" s="150" t="s">
@@ -21040,8 +21043,8 @@
         <v>425</v>
       </c>
       <c r="L45" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-14EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-14EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="M45" s="151" t="s">
         <v>510</v>
@@ -21061,7 +21064,7 @@
         <v>31</v>
       </c>
       <c r="T45" s="153" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB08_ST_614_08_10.val</v>
       </c>
       <c r="U45" s="150" t="s">
@@ -21098,8 +21101,8 @@
       </c>
       <c r="K46" s="150"/>
       <c r="L46" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-0914:AC-PT100-:MeanTemperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-0914:AC-PT100:MeanTemperature-Mon</v>
       </c>
       <c r="M46" s="151" t="s">
         <v>513</v>
@@ -21158,8 +21161,8 @@
         <v>411</v>
       </c>
       <c r="L47" s="221" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-15EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-15EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="M47" s="135" t="s">
         <v>515</v>
@@ -21179,7 +21182,7 @@
         <v>31</v>
       </c>
       <c r="T47" s="177" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB01_ST_614_10_1.val</v>
       </c>
       <c r="U47" s="134" t="s">
@@ -21220,8 +21223,8 @@
         <v>413</v>
       </c>
       <c r="L48" s="221" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-16IW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-16IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="M48" s="135" t="s">
         <v>517</v>
@@ -21241,7 +21244,7 @@
         <v>31</v>
       </c>
       <c r="T48" s="177" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB02_ST_614_10_2.val</v>
       </c>
       <c r="U48" s="134" t="s">
@@ -21282,8 +21285,8 @@
         <v>415</v>
       </c>
       <c r="L49" s="221" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-17IW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-17IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="M49" s="135" t="s">
         <v>519</v>
@@ -21303,7 +21306,7 @@
         <v>31</v>
       </c>
       <c r="T49" s="177" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB03_ST_614_10_4.val</v>
       </c>
       <c r="U49" s="134" t="s">
@@ -21344,8 +21347,8 @@
         <v>417</v>
       </c>
       <c r="L50" s="221" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-17EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-17EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="M50" s="135" t="s">
         <v>521</v>
@@ -21365,7 +21368,7 @@
         <v>31</v>
       </c>
       <c r="T50" s="177" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB04_ST_614_10_5.val</v>
       </c>
       <c r="U50" s="134" t="s">
@@ -21406,8 +21409,8 @@
         <v>419</v>
       </c>
       <c r="L51" s="221" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-18IW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-18IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="M51" s="135" t="s">
         <v>523</v>
@@ -21427,7 +21430,7 @@
         <v>31</v>
       </c>
       <c r="T51" s="177" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB05_ST_614_10_7.val</v>
       </c>
       <c r="U51" s="134" t="s">
@@ -21468,8 +21471,8 @@
         <v>421</v>
       </c>
       <c r="L52" s="221" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-19EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-19EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="M52" s="135" t="s">
         <v>525</v>
@@ -21489,7 +21492,7 @@
         <v>31</v>
       </c>
       <c r="T52" s="177" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB06_ST_614_10_8.val</v>
       </c>
       <c r="U52" s="134" t="s">
@@ -21530,8 +21533,8 @@
         <v>423</v>
       </c>
       <c r="L53" s="221" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-20IW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-20IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="M53" s="135" t="s">
         <v>527</v>
@@ -21551,7 +21554,7 @@
         <v>31</v>
       </c>
       <c r="T53" s="177" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB07_ST_614_10_9.val</v>
       </c>
       <c r="U53" s="134" t="s">
@@ -21592,8 +21595,8 @@
         <v>425</v>
       </c>
       <c r="L54" s="221" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-20EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-20EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="M54" s="135" t="s">
         <v>529</v>
@@ -21613,7 +21616,7 @@
         <v>31</v>
       </c>
       <c r="T54" s="177" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB08_ST_614_10_10.val</v>
       </c>
       <c r="U54" s="134" t="s">
@@ -21650,8 +21653,8 @@
       </c>
       <c r="K55" s="134"/>
       <c r="L55" s="221" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-1520:AC-PT100-:MeanTemperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-1520:AC-PT100:MeanTemperature-Mon</v>
       </c>
       <c r="M55" s="135" t="s">
         <v>531</v>
@@ -21710,8 +21713,8 @@
         <v>411</v>
       </c>
       <c r="L56" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-57IW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-57IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="M56" s="129" t="s">
         <v>533</v>
@@ -21731,7 +21734,7 @@
         <v>31</v>
       </c>
       <c r="T56" s="153" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB01_ST_614_04_1.val</v>
       </c>
       <c r="U56" s="128" t="s">
@@ -21772,8 +21775,8 @@
         <v>413</v>
       </c>
       <c r="L57" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-58EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-58EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="M57" s="129" t="s">
         <v>535</v>
@@ -21793,7 +21796,7 @@
         <v>31</v>
       </c>
       <c r="T57" s="153" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB02_ST_614_04_2.val</v>
       </c>
       <c r="U57" s="128" t="s">
@@ -21834,8 +21837,8 @@
         <v>415</v>
       </c>
       <c r="L58" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-59IW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-59IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="M58" s="129" t="s">
         <v>537</v>
@@ -21855,7 +21858,7 @@
         <v>31</v>
       </c>
       <c r="T58" s="153" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB03_ST_614_04_4.val</v>
       </c>
       <c r="U58" s="128" t="s">
@@ -21896,8 +21899,8 @@
         <v>417</v>
       </c>
       <c r="L59" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-59EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-59EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="M59" s="129" t="s">
         <v>539</v>
@@ -21917,7 +21920,7 @@
         <v>31</v>
       </c>
       <c r="T59" s="153" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB04_ST_614_04_5.val</v>
       </c>
       <c r="U59" s="128" t="s">
@@ -21958,8 +21961,8 @@
         <v>419</v>
       </c>
       <c r="L60" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-60IW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-60IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="M60" s="129" t="s">
         <v>541</v>
@@ -21979,7 +21982,7 @@
         <v>31</v>
       </c>
       <c r="T60" s="153" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB05_ST_614_04_7.val</v>
       </c>
       <c r="U60" s="128" t="s">
@@ -22020,8 +22023,8 @@
         <v>421</v>
       </c>
       <c r="L61" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-01EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-01EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="M61" s="129" t="s">
         <v>543</v>
@@ -22041,7 +22044,7 @@
         <v>31</v>
       </c>
       <c r="T61" s="153" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB06_ST_614_04_8.val</v>
       </c>
       <c r="U61" s="128" t="s">
@@ -22082,8 +22085,8 @@
         <v>423</v>
       </c>
       <c r="L62" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-02IW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-02IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="M62" s="129" t="s">
         <v>545</v>
@@ -22103,7 +22106,7 @@
         <v>31</v>
       </c>
       <c r="T62" s="153" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB07_ST_614_04_9.val</v>
       </c>
       <c r="U62" s="128" t="s">
@@ -22144,8 +22147,8 @@
         <v>425</v>
       </c>
       <c r="L63" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-02EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-02EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="M63" s="129" t="s">
         <v>547</v>
@@ -22165,7 +22168,7 @@
         <v>31</v>
       </c>
       <c r="T63" s="153" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB08_ST_614_04_10.val</v>
       </c>
       <c r="U63" s="128" t="s">
@@ -22202,8 +22205,8 @@
       </c>
       <c r="K64" s="128"/>
       <c r="L64" s="220" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-0160:AC-PT100-:MeanTemperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-0160:AC-PT100:MeanTemperature-Mon</v>
       </c>
       <c r="M64" s="129" t="s">
         <v>550</v>
@@ -22262,8 +22265,8 @@
         <v>411</v>
       </c>
       <c r="L65" s="221" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-03IW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-03IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="M65" s="135" t="s">
         <v>553</v>
@@ -22283,7 +22286,7 @@
         <v>31</v>
       </c>
       <c r="T65" s="177" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB01_ST_614_06_1.val</v>
       </c>
       <c r="U65" s="134" t="s">
@@ -22324,8 +22327,8 @@
         <v>413</v>
       </c>
       <c r="L66" s="221" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-04EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-04EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="M66" s="135" t="s">
         <v>555</v>
@@ -22345,7 +22348,7 @@
         <v>31</v>
       </c>
       <c r="T66" s="177" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB02_ST_614_06_2.val</v>
       </c>
       <c r="U66" s="134" t="s">
@@ -22386,8 +22389,8 @@
         <v>415</v>
       </c>
       <c r="L67" s="221" t="str">
-        <f t="shared" ref="L67:L73" si="2">IF(G67="-",C67&amp;"-"&amp;D67&amp;":"&amp;E67&amp;"-"&amp;F67&amp;":"&amp;H67&amp;"-"&amp;J67,C67&amp;"-"&amp;D67&amp;":"&amp;E67&amp;"-"&amp;F67&amp;"-"&amp;G67&amp;":"&amp;H67&amp;"-"&amp;J67)</f>
-        <v>TU-05IW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-05IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="M67" s="135" t="s">
         <v>557</v>
@@ -22407,7 +22410,7 @@
         <v>31</v>
       </c>
       <c r="T67" s="177" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB03_ST_614_06_4.val</v>
       </c>
       <c r="U67" s="134" t="s">
@@ -22448,8 +22451,8 @@
         <v>417</v>
       </c>
       <c r="L68" s="221" t="str">
-        <f t="shared" si="2"/>
-        <v>TU-05EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-05EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="M68" s="135" t="s">
         <v>559</v>
@@ -22469,7 +22472,7 @@
         <v>31</v>
       </c>
       <c r="T68" s="177" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB04_ST_614_06_5.val</v>
       </c>
       <c r="U68" s="134" t="s">
@@ -22510,8 +22513,8 @@
         <v>419</v>
       </c>
       <c r="L69" s="221" t="str">
-        <f t="shared" si="2"/>
-        <v>TU-06IW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-06IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="M69" s="135" t="s">
         <v>561</v>
@@ -22531,7 +22534,7 @@
         <v>31</v>
       </c>
       <c r="T69" s="177" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB05_ST_614_06_7.val</v>
       </c>
       <c r="U69" s="134" t="s">
@@ -22572,8 +22575,8 @@
         <v>421</v>
       </c>
       <c r="L70" s="221" t="str">
-        <f t="shared" si="2"/>
-        <v>TU-07EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-07EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="M70" s="135" t="s">
         <v>563</v>
@@ -22593,7 +22596,7 @@
         <v>31</v>
       </c>
       <c r="T70" s="177" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB06_ST_614_06_8.val</v>
       </c>
       <c r="U70" s="134" t="s">
@@ -22634,8 +22637,8 @@
         <v>423</v>
       </c>
       <c r="L71" s="221" t="str">
-        <f t="shared" si="2"/>
-        <v>TU-08IW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-08IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="M71" s="135" t="s">
         <v>565</v>
@@ -22655,7 +22658,7 @@
         <v>31</v>
       </c>
       <c r="T71" s="177" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB07_ST_614_06_9.val</v>
       </c>
       <c r="U71" s="134" t="s">
@@ -22696,8 +22699,8 @@
         <v>425</v>
       </c>
       <c r="L72" s="221" t="str">
-        <f t="shared" si="2"/>
-        <v>TU-08EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-08EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="M72" s="135" t="s">
         <v>567</v>
@@ -22717,7 +22720,7 @@
         <v>31</v>
       </c>
       <c r="T72" s="177" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB08_ST_614_06_06.val</v>
       </c>
       <c r="U72" s="134" t="s">
@@ -22735,7 +22738,7 @@
       <c r="C73" s="180" t="s">
         <v>285</v>
       </c>
-      <c r="D73" s="234" t="s">
+      <c r="D73" s="232" t="s">
         <v>569</v>
       </c>
       <c r="E73" s="180" t="s">
@@ -22754,8 +22757,8 @@
       </c>
       <c r="K73" s="180"/>
       <c r="L73" s="221" t="str">
-        <f t="shared" si="2"/>
-        <v>TU-0308:AC-PT100-:MeanTemperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-0308:AC-PT100:MeanTemperature-Mon</v>
       </c>
       <c r="M73" s="181" t="s">
         <v>570</v>
@@ -22792,8 +22795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5C5E429-E963-4A01-A471-5D4A1C2D01BD}">
   <dimension ref="A1:X55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="K47" sqref="K47:K55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -24633,8 +24636,8 @@
         <v>27</v>
       </c>
       <c r="K29" s="223" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-21IW:AC-PT100-:Temperature-Mon</v>
+        <f>IF(G29="-",C29&amp;"-"&amp;D29&amp;":"&amp;E29&amp;"-"&amp;F29&amp;":"&amp;H29&amp;"-"&amp;J29,C29&amp;"-"&amp;D29&amp;":"&amp;E29&amp;"-"&amp;F29&amp;G29&amp;":"&amp;H29&amp;"-"&amp;J29)</f>
+        <v>TU-21IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="L29" s="159" t="s">
         <v>411</v>
@@ -24696,14 +24699,14 @@
         <v>27</v>
       </c>
       <c r="K30" s="223" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-22EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" ref="K30:K37" si="1">IF(G30="-",C30&amp;"-"&amp;D30&amp;":"&amp;E30&amp;"-"&amp;F30&amp;":"&amp;H30&amp;"-"&amp;J30,C30&amp;"-"&amp;D30&amp;":"&amp;E30&amp;"-"&amp;F30&amp;G30&amp;":"&amp;H30&amp;"-"&amp;J30)</f>
+        <v>TU-22EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="L30" s="159" t="s">
         <v>413</v>
       </c>
       <c r="M30" s="129" t="str">
-        <f t="shared" ref="M30:M36" si="1">L30&amp;"_ST_614_"&amp;MID($B30,8,2)&amp;"_"&amp;IF(MID($B30,11,1)="0", MID($B30,12,1), MID($B30,11,2))&amp;".val"</f>
+        <f t="shared" ref="M30:M36" si="2">L30&amp;"_ST_614_"&amp;MID($B30,8,2)&amp;"_"&amp;IF(MID($B30,11,1)="0", MID($B30,12,1), MID($B30,11,2))&amp;".val"</f>
         <v>TEAMB02_ST_614_12_2.val</v>
       </c>
       <c r="N30" s="130" t="s">
@@ -24721,7 +24724,7 @@
         <v>31</v>
       </c>
       <c r="T30" s="132" t="str">
-        <f t="shared" ref="T30:T54" si="2">M30</f>
+        <f t="shared" ref="T30:T54" si="3">M30</f>
         <v>TEAMB02_ST_614_12_2.val</v>
       </c>
       <c r="U30" s="206" t="s">
@@ -24759,14 +24762,14 @@
         <v>27</v>
       </c>
       <c r="K31" s="223" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-23IW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-23IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="L31" s="159" t="s">
         <v>415</v>
       </c>
       <c r="M31" s="129" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB03_ST_614_12_4.val</v>
       </c>
       <c r="N31" s="130" t="s">
@@ -24784,7 +24787,7 @@
         <v>31</v>
       </c>
       <c r="T31" s="132" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TEAMB03_ST_614_12_4.val</v>
       </c>
       <c r="U31" s="206" t="s">
@@ -24822,14 +24825,14 @@
         <v>27</v>
       </c>
       <c r="K32" s="223" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-23EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-23EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="L32" s="159" t="s">
         <v>417</v>
       </c>
       <c r="M32" s="129" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB04_ST_614_12_5.val</v>
       </c>
       <c r="N32" s="130" t="s">
@@ -24847,7 +24850,7 @@
         <v>31</v>
       </c>
       <c r="T32" s="132" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TEAMB04_ST_614_12_5.val</v>
       </c>
       <c r="U32" s="206" t="s">
@@ -24885,14 +24888,14 @@
         <v>27</v>
       </c>
       <c r="K33" s="223" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-24IW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-24IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="L33" s="159" t="s">
         <v>419</v>
       </c>
       <c r="M33" s="129" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB05_ST_614_12_7.val</v>
       </c>
       <c r="N33" s="130" t="s">
@@ -24910,7 +24913,7 @@
         <v>31</v>
       </c>
       <c r="T33" s="132" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TEAMB05_ST_614_12_7.val</v>
       </c>
       <c r="U33" s="206" t="s">
@@ -24948,14 +24951,14 @@
         <v>27</v>
       </c>
       <c r="K34" s="223" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-25EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-25EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="L34" s="159" t="s">
         <v>421</v>
       </c>
       <c r="M34" s="129" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB06_ST_614_12_8.val</v>
       </c>
       <c r="N34" s="130" t="s">
@@ -24973,7 +24976,7 @@
         <v>31</v>
       </c>
       <c r="T34" s="132" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TEAMB06_ST_614_12_8.val</v>
       </c>
       <c r="U34" s="206" t="s">
@@ -25011,14 +25014,14 @@
         <v>27</v>
       </c>
       <c r="K35" s="223" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-26IW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-26IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="L35" s="159" t="s">
         <v>423</v>
       </c>
       <c r="M35" s="129" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB07_ST_614_12_9.val</v>
       </c>
       <c r="N35" s="130" t="s">
@@ -25036,7 +25039,7 @@
         <v>31</v>
       </c>
       <c r="T35" s="132" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TEAMB07_ST_614_12_9.val</v>
       </c>
       <c r="U35" s="206" t="s">
@@ -25074,14 +25077,14 @@
         <v>27</v>
       </c>
       <c r="K36" s="223" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-26EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-26EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="L36" s="159" t="s">
         <v>425</v>
       </c>
       <c r="M36" s="129" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TEAMB08_ST_614_12_10.val</v>
       </c>
       <c r="N36" s="130" t="s">
@@ -25099,7 +25102,7 @@
         <v>31</v>
       </c>
       <c r="T36" s="132" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TEAMB08_ST_614_12_10.val</v>
       </c>
       <c r="U36" s="206" t="s">
@@ -25135,8 +25138,8 @@
         <v>27</v>
       </c>
       <c r="K37" s="223" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-2126:AC-PT100-:MeanTemperature-Mon</v>
+        <f t="shared" si="1"/>
+        <v>TU-2126:AC-PT100:MeanTemperature-Mon</v>
       </c>
       <c r="L37" s="159"/>
       <c r="M37" s="129" t="s">
@@ -25193,8 +25196,8 @@
         <v>27</v>
       </c>
       <c r="K38" s="224" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-27IW:AC-PT100-:Temperature-Mon</v>
+        <f>IF(G38="-",C38&amp;"-"&amp;D38&amp;":"&amp;E38&amp;"-"&amp;F38&amp;":"&amp;H38&amp;"-"&amp;J38,C38&amp;"-"&amp;D38&amp;":"&amp;E38&amp;"-"&amp;F38&amp;G38&amp;":"&amp;H38&amp;"-"&amp;J38)</f>
+        <v>TU-27IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="L38" s="160" t="s">
         <v>411</v>
@@ -25256,14 +25259,14 @@
         <v>27</v>
       </c>
       <c r="K39" s="224" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-28EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" ref="K39:K46" si="4">IF(G39="-",C39&amp;"-"&amp;D39&amp;":"&amp;E39&amp;"-"&amp;F39&amp;":"&amp;H39&amp;"-"&amp;J39,C39&amp;"-"&amp;D39&amp;":"&amp;E39&amp;"-"&amp;F39&amp;G39&amp;":"&amp;H39&amp;"-"&amp;J39)</f>
+        <v>TU-28EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="L39" s="160" t="s">
         <v>413</v>
       </c>
       <c r="M39" s="135" t="str">
-        <f t="shared" ref="M39:M45" si="3">L39&amp;"_ST_614_"&amp;MID($B39,8,2)&amp;"_"&amp;IF(MID($B39,11,1)="0", MID($B39,12,1), MID($B39,11,2))&amp;".val"</f>
+        <f t="shared" ref="M39:M45" si="5">L39&amp;"_ST_614_"&amp;MID($B39,8,2)&amp;"_"&amp;IF(MID($B39,11,1)="0", MID($B39,12,1), MID($B39,11,2))&amp;".val"</f>
         <v>TEAMB02_ST_614_14_2.val</v>
       </c>
       <c r="N39" s="136" t="s">
@@ -25319,14 +25322,14 @@
         <v>27</v>
       </c>
       <c r="K40" s="224" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-29IW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="4"/>
+        <v>TU-29IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="L40" s="160" t="s">
         <v>415</v>
       </c>
       <c r="M40" s="135" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>TEAMB03_ST_614_14_4.val</v>
       </c>
       <c r="N40" s="136" t="s">
@@ -25382,14 +25385,14 @@
         <v>27</v>
       </c>
       <c r="K41" s="224" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-29EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="4"/>
+        <v>TU-29EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="L41" s="160" t="s">
         <v>417</v>
       </c>
       <c r="M41" s="135" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>TEAMB04_ST_614_14_5.val</v>
       </c>
       <c r="N41" s="136" t="s">
@@ -25445,14 +25448,14 @@
         <v>27</v>
       </c>
       <c r="K42" s="224" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-30IW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="4"/>
+        <v>TU-30IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="L42" s="160" t="s">
         <v>419</v>
       </c>
       <c r="M42" s="135" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>TEAMB05_ST_614_14_7.val</v>
       </c>
       <c r="N42" s="136" t="s">
@@ -25508,14 +25511,14 @@
         <v>27</v>
       </c>
       <c r="K43" s="224" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-31EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="4"/>
+        <v>TU-31EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="L43" s="160" t="s">
         <v>421</v>
       </c>
       <c r="M43" s="135" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>TEAMB06_ST_614_14_8.val</v>
       </c>
       <c r="N43" s="136" t="s">
@@ -25571,14 +25574,14 @@
         <v>27</v>
       </c>
       <c r="K44" s="224" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-32IW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="4"/>
+        <v>TU-32IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="L44" s="160" t="s">
         <v>423</v>
       </c>
       <c r="M44" s="135" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>TEAMB07_ST_614_14_9.val</v>
       </c>
       <c r="N44" s="136" t="s">
@@ -25634,14 +25637,14 @@
         <v>27</v>
       </c>
       <c r="K45" s="224" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-32EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="4"/>
+        <v>TU-32EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="L45" s="160" t="s">
         <v>425</v>
       </c>
       <c r="M45" s="135" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>TEAMB08_ST_614_14_10.val</v>
       </c>
       <c r="N45" s="136" t="s">
@@ -25695,8 +25698,8 @@
         <v>27</v>
       </c>
       <c r="K46" s="224" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-2732:AC-PT100-:MeanTemperature-Mon</v>
+        <f t="shared" si="4"/>
+        <v>TU-2732:AC-PT100:MeanTemperature-Mon</v>
       </c>
       <c r="L46" s="160"/>
       <c r="M46" s="135" t="s">
@@ -25753,8 +25756,8 @@
         <v>27</v>
       </c>
       <c r="K47" s="223" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-33IW:AC-PT100-:Temperature-Mon</v>
+        <f>IF(G47="-",C47&amp;"-"&amp;D47&amp;":"&amp;E47&amp;"-"&amp;F47&amp;":"&amp;H47&amp;"-"&amp;J47,C47&amp;"-"&amp;D47&amp;":"&amp;E47&amp;"-"&amp;F47&amp;G47&amp;":"&amp;H47&amp;"-"&amp;J47)</f>
+        <v>TU-33IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="L47" s="159" t="s">
         <v>411</v>
@@ -25778,7 +25781,7 @@
         <v>31</v>
       </c>
       <c r="T47" s="132" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TEAMB01_ST_614_16_1.val</v>
       </c>
       <c r="U47" s="229" t="s">
@@ -25816,14 +25819,14 @@
         <v>27</v>
       </c>
       <c r="K48" s="223" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-34EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" ref="K48:K55" si="6">IF(G48="-",C48&amp;"-"&amp;D48&amp;":"&amp;E48&amp;"-"&amp;F48&amp;":"&amp;H48&amp;"-"&amp;J48,C48&amp;"-"&amp;D48&amp;":"&amp;E48&amp;"-"&amp;F48&amp;G48&amp;":"&amp;H48&amp;"-"&amp;J48)</f>
+        <v>TU-34EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="L48" s="159" t="s">
         <v>413</v>
       </c>
       <c r="M48" s="129" t="str">
-        <f t="shared" ref="M48:M54" si="4">L48&amp;"_ST_614_"&amp;MID($B48,8,2)&amp;"_"&amp;IF(MID($B48,11,1)="0", MID($B48,12,1), MID($B48,11,2))&amp;".val"</f>
+        <f t="shared" ref="M48:M54" si="7">L48&amp;"_ST_614_"&amp;MID($B48,8,2)&amp;"_"&amp;IF(MID($B48,11,1)="0", MID($B48,12,1), MID($B48,11,2))&amp;".val"</f>
         <v>TEAMB02_ST_614_16_2.val</v>
       </c>
       <c r="N48" s="130" t="s">
@@ -25841,7 +25844,7 @@
         <v>31</v>
       </c>
       <c r="T48" s="132" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TEAMB02_ST_614_16_2.val</v>
       </c>
       <c r="U48" s="206" t="s">
@@ -25879,14 +25882,14 @@
         <v>27</v>
       </c>
       <c r="K49" s="223" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-35IW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="6"/>
+        <v>TU-35IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="L49" s="159" t="s">
         <v>415</v>
       </c>
       <c r="M49" s="129" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>TEAMB03_ST_614_16_4.val</v>
       </c>
       <c r="N49" s="130" t="s">
@@ -25904,7 +25907,7 @@
         <v>31</v>
       </c>
       <c r="T49" s="132" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TEAMB03_ST_614_16_4.val</v>
       </c>
       <c r="U49" s="206" t="s">
@@ -25942,14 +25945,14 @@
         <v>27</v>
       </c>
       <c r="K50" s="223" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-35EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="6"/>
+        <v>TU-35EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="L50" s="159" t="s">
         <v>417</v>
       </c>
       <c r="M50" s="129" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>TEAMB04_ST_614_16_5.val</v>
       </c>
       <c r="N50" s="130" t="s">
@@ -25967,7 +25970,7 @@
         <v>31</v>
       </c>
       <c r="T50" s="132" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TEAMB04_ST_614_16_5.val</v>
       </c>
       <c r="U50" s="206" t="s">
@@ -26005,14 +26008,14 @@
         <v>27</v>
       </c>
       <c r="K51" s="223" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-36IW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="6"/>
+        <v>TU-36IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="L51" s="159" t="s">
         <v>419</v>
       </c>
       <c r="M51" s="129" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>TEAMB05_ST_614_16_7.val</v>
       </c>
       <c r="N51" s="130" t="s">
@@ -26030,7 +26033,7 @@
         <v>31</v>
       </c>
       <c r="T51" s="132" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TEAMB05_ST_614_16_7.val</v>
       </c>
       <c r="U51" s="206" t="s">
@@ -26068,14 +26071,14 @@
         <v>27</v>
       </c>
       <c r="K52" s="223" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-37EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="6"/>
+        <v>TU-37EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="L52" s="159" t="s">
         <v>421</v>
       </c>
       <c r="M52" s="129" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>TEAMB06_ST_614_16_8.val</v>
       </c>
       <c r="N52" s="130" t="s">
@@ -26093,7 +26096,7 @@
         <v>31</v>
       </c>
       <c r="T52" s="132" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TEAMB06_ST_614_16_8.val</v>
       </c>
       <c r="U52" s="206" t="s">
@@ -26131,14 +26134,14 @@
         <v>27</v>
       </c>
       <c r="K53" s="223" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-38IW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="6"/>
+        <v>TU-38IW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="L53" s="159" t="s">
         <v>423</v>
       </c>
       <c r="M53" s="129" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>TEAMB07_ST_614_16_9.val</v>
       </c>
       <c r="N53" s="130" t="s">
@@ -26156,7 +26159,7 @@
         <v>31</v>
       </c>
       <c r="T53" s="132" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TEAMB07_ST_614_16_9.val</v>
       </c>
       <c r="U53" s="206" t="s">
@@ -26194,14 +26197,14 @@
         <v>27</v>
       </c>
       <c r="K54" s="223" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-38EW:AC-PT100-:Temperature-Mon</v>
+        <f t="shared" si="6"/>
+        <v>TU-38EW:AC-PT100:Temperature-Mon</v>
       </c>
       <c r="L54" s="189" t="s">
         <v>425</v>
       </c>
       <c r="M54" s="190" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>TEAMB08_ST_614_16_10.val</v>
       </c>
       <c r="N54" s="191" t="s">
@@ -26219,7 +26222,7 @@
         <v>31</v>
       </c>
       <c r="T54" s="194" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TEAMB08_ST_614_16_10.val</v>
       </c>
       <c r="U54" s="211" t="s">
@@ -26255,8 +26258,8 @@
         <v>27</v>
       </c>
       <c r="K55" s="223" t="str">
-        <f t="shared" si="0"/>
-        <v>TU-3338:AC-PT100-:MeanTemperature-Mon</v>
+        <f t="shared" si="6"/>
+        <v>TU-3338:AC-PT100:MeanTemperature-Mon</v>
       </c>
       <c r="L55" s="196"/>
       <c r="M55" s="197" t="s">
@@ -26326,11 +26329,11 @@
       <c r="F1" s="45" t="s">
         <v>641</v>
       </c>
-      <c r="H1" s="233" t="s">
+      <c r="H1" s="234" t="s">
         <v>639</v>
       </c>
-      <c r="I1" s="233"/>
-      <c r="J1" s="232" t="s">
+      <c r="I1" s="234"/>
+      <c r="J1" s="233" t="s">
         <v>641</v>
       </c>
     </row>
@@ -26360,7 +26363,7 @@
       <c r="I2" s="45" t="s">
         <v>644</v>
       </c>
-      <c r="J2" s="232"/>
+      <c r="J2" s="233"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="45" t="str">
@@ -28275,34 +28278,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="ed202a06-a5fd-4989-ab35-516afb994abd">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <MediaLengthInSeconds xmlns="b2c2e3a4-82bc-4b14-ba75-76c6e4b67a60" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b2c2e3a4-82bc-4b14-ba75-76c6e4b67a60">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="ed202a06-a5fd-4989-ab35-516afb994abd" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101006F4FA476A4A600469C08194709EC5E9A" ma:contentTypeVersion="16" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="fd3d69f9800133fc7e273e7f140e322c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b2c2e3a4-82bc-4b14-ba75-76c6e4b67a60" xmlns:ns3="ed202a06-a5fd-4989-ab35-516afb994abd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3e9c683e6dadc058b32391737b115ac4" ns2:_="" ns3:_="">
     <xsd:import namespace="b2c2e3a4-82bc-4b14-ba75-76c6e4b67a60"/>
@@ -28545,8 +28520,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="ed202a06-a5fd-4989-ab35-516afb994abd">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <MediaLengthInSeconds xmlns="b2c2e3a4-82bc-4b14-ba75-76c6e4b67a60" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b2c2e3a4-82bc-4b14-ba75-76c6e4b67a60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="ed202a06-a5fd-4989-ab35-516afb994abd" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F73AECD0-D97F-4072-8B5A-ACBE5E9143A8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37CAFCCB-79BC-46EE-B295-ED437D5AD1F9}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -28554,5 +28557,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37CAFCCB-79BC-46EE-B295-ED437D5AD1F9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F73AECD0-D97F-4072-8B5A-ACBE5E9143A8}"/>
 </file>
</xml_diff>